<commit_message>
se implementa filtro (no funcional)
</commit_message>
<xml_diff>
--- a/src/assets/archivos/Plantilla_estandar_para_cargar_bienes.xlsx
+++ b/src/assets/archivos/Plantilla_estandar_para_cargar_bienes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B2AB36F3-C412-473A-8E7B-67C41EC5AE40}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B7FF00A-74D7-4CA4-B485-BF969FA01D90}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{76B2D214-ADFE-4F4A-AF10-639C5440C757}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Bienes</t>
   </si>
@@ -55,9 +55,6 @@
     <t>Valor estimado</t>
   </si>
   <si>
-    <t>Centro de costos/ Orden de inversión</t>
-  </si>
-  <si>
     <t>Tipo de moneda</t>
   </si>
   <si>
@@ -104,6 +101,12 @@
   </si>
   <si>
     <t>Orden de inversión</t>
+  </si>
+  <si>
+    <t>ID de Servicios</t>
+  </si>
+  <si>
+    <t>Centro de costos/ Orden de inversión/ ID de Servicios</t>
   </si>
 </sst>
 </file>
@@ -194,11 +197,11 @@
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Encabezado 1" xfId="1" builtinId="16"/>
@@ -517,8 +520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F36E9134-462E-4DCA-BA2C-4DBF27E15D3F}">
   <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -526,26 +529,26 @@
     <col min="1" max="1" width="26.140625" customWidth="1"/>
     <col min="2" max="2" width="38.5703125" customWidth="1"/>
     <col min="6" max="7" width="20.5703125" customWidth="1"/>
-    <col min="8" max="8" width="39.28515625" customWidth="1"/>
+    <col min="8" max="8" width="64.7109375" customWidth="1"/>
     <col min="9" max="9" width="52.85546875" customWidth="1"/>
     <col min="10" max="10" width="20.42578125" customWidth="1"/>
     <col min="11" max="11" width="23.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="34.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
     </row>
     <row r="2" spans="1:12" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
@@ -567,26 +570,26 @@
         <v>6</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="1" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="3" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="F3" s="3"/>
+      <c r="F3" s="2"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="L10" s="4"/>
+      <c r="L10" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -603,11 +606,11 @@
           </x14:formula1>
           <xm:sqref>G3:G102</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Seleccione" xr:uid="{689872E2-9221-4C5D-979A-9E50F0F40944}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Seleccione" xr:uid="{0A06E92B-995E-4A28-A6AB-3C9074BA1552}">
           <x14:formula1>
-            <xm:f>Desplegables!$B$2:$B$3</xm:f>
+            <xm:f>Desplegables!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>H3:H102</xm:sqref>
+          <xm:sqref>H3:H327</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -620,7 +623,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -631,56 +634,59 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se modifican plantillas de excel
</commit_message>
<xml_diff>
--- a/src/assets/archivos/Plantilla_estandar_para_cargar_bienes.xlsx
+++ b/src/assets/archivos/Plantilla_estandar_para_cargar_bienes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B7FF00A-74D7-4CA4-B485-BF969FA01D90}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59F76AB5-CCF9-4B1A-A384-36A9564FBE75}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{76B2D214-ADFE-4F4A-AF10-639C5440C757}"/>
   </bookViews>
@@ -58,9 +58,6 @@
     <t>Tipo de moneda</t>
   </si>
   <si>
-    <t>Número de centro de costos/ Orden de inversión</t>
-  </si>
-  <si>
     <t>Número de cuenta</t>
   </si>
   <si>
@@ -107,6 +104,9 @@
   </si>
   <si>
     <t>Centro de costos/ Orden de inversión/ ID de Servicios</t>
+  </si>
+  <si>
+    <t>Número de centro de costos/ Orden de inversión/ ID de Servicios</t>
   </si>
 </sst>
 </file>
@@ -520,8 +520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F36E9134-462E-4DCA-BA2C-4DBF27E15D3F}">
   <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -529,8 +529,8 @@
     <col min="1" max="1" width="26.140625" customWidth="1"/>
     <col min="2" max="2" width="38.5703125" customWidth="1"/>
     <col min="6" max="7" width="20.5703125" customWidth="1"/>
-    <col min="8" max="8" width="64.7109375" customWidth="1"/>
-    <col min="9" max="9" width="52.85546875" customWidth="1"/>
+    <col min="8" max="8" width="57.140625" customWidth="1"/>
+    <col min="9" max="9" width="69.85546875" customWidth="1"/>
     <col min="10" max="10" width="20.42578125" customWidth="1"/>
     <col min="11" max="11" width="23.140625" customWidth="1"/>
   </cols>
@@ -573,16 +573,16 @@
         <v>7</v>
       </c>
       <c r="H2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -634,59 +634,59 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se agregan plantillas actualizadas
</commit_message>
<xml_diff>
--- a/src/assets/archivos/Plantilla_estandar_para_cargar_bienes.xlsx
+++ b/src/assets/archivos/Plantilla_estandar_para_cargar_bienes.xlsx
@@ -692,4 +692,163 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010065AB61EBD1D26542B2E280FFA53CD654" ma:contentTypeVersion="2" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="696e21d476276e33d779ddb2bc4f66de">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="84e1c395-7d59-405d-ad96-8ad5fd8aa952" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="effc6c0671f8dfb4066fda915563918b" ns2:_="">
+    <xsd:import namespace="84e1c395-7d59-405d-ad96-8ad5fd8aa952"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="84e1c395-7d59-405d-ad96-8ad5fd8aa952" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Tipo de contenido"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Título"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{24B192E9-FFD1-4387-9B87-4A2D31530753}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1E84187F-6B22-479E-8DB7-289418D8192C}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1841DDF8-D7DD-45C9-867A-E89536147B35}"/>
 </file>
</xml_diff>